<commit_message>
scalar data type and attributes are remaining
</commit_message>
<xml_diff>
--- a/2-FPGA-designs-with-VHDL/Chapters/Datatypes/Figures/VHDLoperators.xlsx
+++ b/2-FPGA-designs-with-VHDL/Chapters/Datatypes/Figures/VHDLoperators.xlsx
@@ -11,12 +11,15 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="76">
   <si>
     <t>Type</t>
   </si>
@@ -117,9 +120,6 @@
     <t>Boolean</t>
   </si>
   <si>
-    <t>a ** b</t>
-  </si>
-  <si>
     <t>a &gt; b</t>
   </si>
   <si>
@@ -162,51 +162,91 @@
     <t>integer, natural, positive, signed and unsigned</t>
   </si>
   <si>
-    <t>power (natural, positive, constant positive integer)</t>
-  </si>
-  <si>
-    <t>c (exactly 9 bit i.e. 4+5) = a * b</t>
-  </si>
-  <si>
-    <t>c (exactly 5 bit) = a - b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c (exactly 5 bit) = a + b </t>
-  </si>
-  <si>
     <t xml:space="preserve">  '0' &amp; "101" = "0101"</t>
   </si>
   <si>
-    <r>
-      <t>c (exactly 5 bit)=a / b (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>may not synthesize</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve"> "101" &amp; '0'  &amp; "11"= "101011"</t>
   </si>
   <si>
     <t>can be used for shift operations</t>
+  </si>
+  <si>
+    <t>mod</t>
+  </si>
+  <si>
+    <t>integer, natural,  positive</t>
+  </si>
+  <si>
+    <t>rem</t>
+  </si>
+  <si>
+    <t>a mod b (returns remainder with sign of b)</t>
+  </si>
+  <si>
+    <t>abs</t>
+  </si>
+  <si>
+    <t>natural, positive, constant positive integer</t>
+  </si>
+  <si>
+    <t>a ** b (e.g. 2**3 = 8)</t>
+  </si>
+  <si>
+    <t>c (exactly 5 bit) = a + b (if a and b are signed/unsigned)</t>
+  </si>
+  <si>
+    <t>c (exactly 5 bit) = a - b (if a and b are signed/unsigned)</t>
+  </si>
+  <si>
+    <t>c (exactly 9 bit i.e. 4+5) = a * b (if a and b are signed/unsigned)</t>
+  </si>
+  <si>
+    <t>c (exactly 5 bit)=a / b (if a and b are signed/unsigned &amp;                                                         ignores the decimal values e.g. 5/-2 =  -2)</t>
+  </si>
+  <si>
+    <t>abs(a)  (absolute value of a)</t>
+  </si>
+  <si>
+    <t>a rem b (returns remainder with sign of a)</t>
+  </si>
+  <si>
+    <t>Assignment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> :=</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  =&gt;</t>
+  </si>
+  <si>
+    <t>a &lt;= "1001"</t>
+  </si>
+  <si>
+    <t>b := "1001"</t>
+  </si>
+  <si>
+    <t>assign initial value of signals and variables</t>
+  </si>
+  <si>
+    <t>signal a : std_logic := '1'</t>
+  </si>
+  <si>
+    <t>variable a : std_logic := '1'</t>
+  </si>
+  <si>
+    <t>assign value to variable</t>
+  </si>
+  <si>
+    <t>assign value to singal</t>
+  </si>
+  <si>
+    <t>assign value using 'others'</t>
+  </si>
+  <si>
+    <t>a &lt;= (others =&gt; '0')</t>
   </si>
 </sst>
 </file>
@@ -316,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -324,33 +364,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -362,13 +402,50 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -664,10 +741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,274 +752,374 @@
     <col min="1" max="1" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="39.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.7109375" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>46</v>
+      <c r="D1" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>51</v>
+      <c r="C2" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="15"/>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="7" t="s">
-        <v>50</v>
+      <c r="C3" s="10"/>
+      <c r="D3" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="7" t="s">
-        <v>49</v>
+      <c r="C4" s="10"/>
+      <c r="D4" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>33</v>
-      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>27</v>
+      <c r="A7" s="15"/>
+      <c r="B7" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
-      <c r="B8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>28</v>
+      <c r="B8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
-      <c r="B9" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>29</v>
+      <c r="B9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>41</v>
+      <c r="A11" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
-      <c r="B12" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>30</v>
+      <c r="B12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>45</v>
+      <c r="A13" s="15"/>
+      <c r="B13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>34</v>
+      <c r="A14" s="15"/>
+      <c r="B14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
-      <c r="B15" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>35</v>
+      <c r="B15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="B19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+      <c r="B20" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C20" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D20" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="B21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="7" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
+      <c r="B22" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="7" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B24" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="11" t="s">
-        <v>54</v>
+      <c r="C24" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="17"/>
+      <c r="B27" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="17"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="17"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="18"/>
+      <c r="B30" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A13"/>
-    <mergeCell ref="A14:A19"/>
+  <mergeCells count="13">
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="A11:A17"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="8" orientation="portrait" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>